<commit_message>
Added new HARWIN connector to list
</commit_message>
<xml_diff>
--- a/hardware/component-info.xlsx
+++ b/hardware/component-info.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Component</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>http://uk.farnell.com/fci/20021321-00016c4lf/receptacle-vert-1-27mm-smt-16way/dp/1865311?Ntt=20021321-00016C4LF</t>
+  </si>
+  <si>
+    <t>HARWIN</t>
+  </si>
+  <si>
+    <t>M20-7870842</t>
+  </si>
+  <si>
+    <t>http://www.harwin.com/search/M20-7870842?ProductSearch=True</t>
   </si>
 </sst>
 </file>
@@ -455,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -584,13 +593,34 @@
         <v>25</v>
       </c>
     </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I3" r:id="rId1"/>
     <hyperlink ref="I4" r:id="rId2"/>
+    <hyperlink ref="I5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>